<commit_message>
Amended metrics (SDG update)
</commit_message>
<xml_diff>
--- a/translations/en/Global Indicator Framework after refinement.English.xlsx
+++ b/translations/en/Global Indicator Framework after refinement.English.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="420" windowWidth="21580" windowHeight="23120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="A.RES.71.313 Annex" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>Metrics overview</t>
   </si>
   <si>
-    <t>Areas and Topics</t>
-  </si>
-  <si>
     <t>7.1 Population</t>
   </si>
   <si>
@@ -378,6 +375,9 @@
   </si>
   <si>
     <t>7.1.3 Population growth projections</t>
+  </si>
+  <si>
+    <t>Areas and Targets</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1085,7 +1085,7 @@
     <row r="3" spans="1:3">
       <c r="A3" s="2"/>
       <c r="B3" s="12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>108</v>
@@ -1730,20 +1730,20 @@
     <row r="88" spans="1:3">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="C89" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="C90" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>